<commit_message>
Añadido datos a INDIVIDUAL.xlsx
</commit_message>
<xml_diff>
--- a/Datos/INDIVIDUAL.xlsx
+++ b/Datos/INDIVIDUAL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\Datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\javie\Desktop\UNIVERSIDAD\TERCERO\2_Administración-bases-de-datos\Trabajo-grupo\ABD\Datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{822337A7-D996-4B3B-8D86-046C715EE779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F2C196A-7368-4FCE-841A-0A7D77355B96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -43,6 +43,30 @@
   </si>
   <si>
     <t>Pérez</t>
+  </si>
+  <si>
+    <t>Antón</t>
+  </si>
+  <si>
+    <t>Torrón</t>
+  </si>
+  <si>
+    <t>Xin</t>
+  </si>
+  <si>
+    <t>Lú</t>
+  </si>
+  <si>
+    <t>Belén</t>
+  </si>
+  <si>
+    <t>Pastor Iglesias</t>
+  </si>
+  <si>
+    <t>Aitor</t>
+  </si>
+  <si>
+    <t>Menta</t>
   </si>
 </sst>
 </file>
@@ -360,15 +384,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -397,6 +421,50 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>